<commit_message>
Updated to Nov 14 2022
</commit_message>
<xml_diff>
--- a/data/SerieA_22_23_goal_spread.xlsx
+++ b/data/SerieA_22_23_goal_spread.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="47">
   <si>
     <t xml:space="preserve">giornata</t>
   </si>
@@ -343,7 +343,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,6 +414,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -503,13 +507,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB241"/>
+  <dimension ref="A1:AB302"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="C:C H:H"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A282" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K291" activeCellId="0" sqref="K291"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.8"/>
@@ -15767,6 +15771,3609 @@
       <c r="AA241" s="15"/>
       <c r="AB241" s="17"/>
     </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="10" t="n">
+        <v>13</v>
+      </c>
+      <c r="B242" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H242" s="2" t="n">
+        <f aca="false">60</f>
+        <v>60</v>
+      </c>
+      <c r="I242" s="1" t="n">
+        <f aca="false">0.28</f>
+        <v>0.28</v>
+      </c>
+      <c r="J242" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="K242" s="1" t="n">
+        <f aca="false">0.72</f>
+        <v>0.72</v>
+      </c>
+      <c r="L242" s="1" t="n">
+        <f aca="false">7</f>
+        <v>7</v>
+      </c>
+      <c r="M242" s="2" t="n">
+        <f aca="false">19+12</f>
+        <v>31</v>
+      </c>
+      <c r="N242" s="1" t="n">
+        <f aca="false">0+0.29</f>
+        <v>0.29</v>
+      </c>
+      <c r="O242" s="1" t="n">
+        <f aca="false">0+2</f>
+        <v>2</v>
+      </c>
+      <c r="P242" s="1" t="n">
+        <f aca="false">0.42+0.1</f>
+        <v>0.52</v>
+      </c>
+      <c r="Q242" s="1" t="n">
+        <f aca="false">6+2</f>
+        <v>8</v>
+      </c>
+      <c r="R242" s="2" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="S242" s="1" t="n">
+        <f aca="false">0.42</f>
+        <v>0.42</v>
+      </c>
+      <c r="T242" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="U242" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="V242" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H243" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="I243" s="1" t="n">
+        <f aca="false">0.24</f>
+        <v>0.24</v>
+      </c>
+      <c r="J243" s="1" t="n">
+        <f aca="false">5</f>
+        <v>5</v>
+      </c>
+      <c r="K243" s="1" t="n">
+        <f aca="false">0.45</f>
+        <v>0.45</v>
+      </c>
+      <c r="L243" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="M243" s="2" t="n">
+        <f aca="false">26+9</f>
+        <v>35</v>
+      </c>
+      <c r="N243" s="1" t="n">
+        <f aca="false">0+0</f>
+        <v>0</v>
+      </c>
+      <c r="O243" s="1" t="n">
+        <f aca="false">0+0</f>
+        <v>0</v>
+      </c>
+      <c r="P243" s="1" t="n">
+        <f aca="false">0.57+0.49</f>
+        <v>1.06</v>
+      </c>
+      <c r="Q243" s="1" t="n">
+        <f aca="false">3+2</f>
+        <v>5</v>
+      </c>
+      <c r="R243" s="2" t="n">
+        <f aca="false">25</f>
+        <v>25</v>
+      </c>
+      <c r="S243" s="1" t="n">
+        <f aca="false">0.02</f>
+        <v>0.02</v>
+      </c>
+      <c r="T243" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="U243" s="1" t="n">
+        <f aca="false">0.46</f>
+        <v>0.46</v>
+      </c>
+      <c r="V243" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H244" s="2" t="n">
+        <f aca="false">R256</f>
+        <v>60</v>
+      </c>
+      <c r="I244" s="1" t="n">
+        <f aca="false">U256</f>
+        <v>0.08</v>
+      </c>
+      <c r="J244" s="1" t="n">
+        <f aca="false">V256</f>
+        <v>1</v>
+      </c>
+      <c r="K244" s="1" t="n">
+        <f aca="false">S256</f>
+        <v>0.62</v>
+      </c>
+      <c r="L244" s="1" t="n">
+        <f aca="false">T256</f>
+        <v>6</v>
+      </c>
+      <c r="M244" s="2" t="n">
+        <f aca="false">M256</f>
+        <v>39</v>
+      </c>
+      <c r="N244" s="1" t="n">
+        <f aca="false">P256</f>
+        <v>1.21</v>
+      </c>
+      <c r="O244" s="1" t="n">
+        <f aca="false">Q256</f>
+        <v>7</v>
+      </c>
+      <c r="P244" s="1" t="n">
+        <f aca="false">N256</f>
+        <v>0.17</v>
+      </c>
+      <c r="Q244" s="1" t="n">
+        <f aca="false">O256</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M245" s="2" t="n">
+        <f aca="false">64</f>
+        <v>64</v>
+      </c>
+      <c r="N245" s="1" t="n">
+        <f aca="false">0.09</f>
+        <v>0.09</v>
+      </c>
+      <c r="O245" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="P245" s="1" t="n">
+        <f aca="false">0.84</f>
+        <v>0.84</v>
+      </c>
+      <c r="Q245" s="1" t="n">
+        <f aca="false">14</f>
+        <v>14</v>
+      </c>
+      <c r="R245" s="2" t="n">
+        <f aca="false">32</f>
+        <v>32</v>
+      </c>
+      <c r="S245" s="1" t="n">
+        <f aca="false">0.47</f>
+        <v>0.47</v>
+      </c>
+      <c r="T245" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="U245" s="1" t="n">
+        <f aca="false">0.38</f>
+        <v>0.38</v>
+      </c>
+      <c r="V245" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M246" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N246" s="1" t="n">
+        <f aca="false">P257</f>
+        <v>0.12</v>
+      </c>
+      <c r="O246" s="1" t="n">
+        <f aca="false">Q257</f>
+        <v>1</v>
+      </c>
+      <c r="P246" s="1" t="n">
+        <f aca="false">N257</f>
+        <v>0.17</v>
+      </c>
+      <c r="Q246" s="1" t="n">
+        <f aca="false">O257</f>
+        <v>1</v>
+      </c>
+      <c r="R246" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="S246" s="1" t="n">
+        <f aca="false">K257</f>
+        <v>0.59</v>
+      </c>
+      <c r="T246" s="1" t="n">
+        <f aca="false">L257</f>
+        <v>10</v>
+      </c>
+      <c r="U246" s="1" t="n">
+        <f aca="false">I257</f>
+        <v>0.64</v>
+      </c>
+      <c r="V246" s="1" t="n">
+        <f aca="false">J257</f>
+        <v>3</v>
+      </c>
+      <c r="W246" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="X246" s="1" t="n">
+        <f aca="false">F257</f>
+        <v>0.07</v>
+      </c>
+      <c r="Y246" s="1" t="n">
+        <f aca="false">G257</f>
+        <v>3</v>
+      </c>
+      <c r="Z246" s="1" t="n">
+        <f aca="false">D257</f>
+        <v>0.09</v>
+      </c>
+      <c r="AA246" s="1" t="n">
+        <f aca="false">E257</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C247" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D247" s="1" t="n">
+        <f aca="false">Z253</f>
+        <v>0.06</v>
+      </c>
+      <c r="E247" s="1" t="n">
+        <f aca="false">AA253</f>
+        <v>1</v>
+      </c>
+      <c r="F247" s="1" t="n">
+        <f aca="false">X253</f>
+        <v>0.06</v>
+      </c>
+      <c r="G247" s="1" t="n">
+        <f aca="false">Y253</f>
+        <v>2</v>
+      </c>
+      <c r="H247" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I247" s="1" t="n">
+        <f aca="false">U253</f>
+        <v>0.26</v>
+      </c>
+      <c r="J247" s="1" t="n">
+        <f aca="false">V253</f>
+        <v>4</v>
+      </c>
+      <c r="K247" s="1" t="n">
+        <f aca="false">S253</f>
+        <v>0.01</v>
+      </c>
+      <c r="L247" s="1" t="n">
+        <f aca="false">T253</f>
+        <v>1</v>
+      </c>
+      <c r="M247" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="N247" s="1" t="n">
+        <f aca="false">P253</f>
+        <v>0.83</v>
+      </c>
+      <c r="O247" s="1" t="n">
+        <f aca="false">Q253</f>
+        <v>8</v>
+      </c>
+      <c r="P247" s="1" t="n">
+        <f aca="false">N253</f>
+        <v>0.29</v>
+      </c>
+      <c r="Q247" s="1" t="n">
+        <f aca="false">O253</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M248" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="N248" s="1" t="n">
+        <f aca="false">0.84</f>
+        <v>0.84</v>
+      </c>
+      <c r="O248" s="1" t="n">
+        <f aca="false">8</f>
+        <v>8</v>
+      </c>
+      <c r="P248" s="1" t="n">
+        <f aca="false">0.69</f>
+        <v>0.69</v>
+      </c>
+      <c r="Q248" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="R248" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="S248" s="1" t="n">
+        <f aca="false">0.32</f>
+        <v>0.32</v>
+      </c>
+      <c r="T248" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="U248" s="1" t="n">
+        <f aca="false">0.23</f>
+        <v>0.23</v>
+      </c>
+      <c r="V248" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="W248" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="X248" s="1" t="n">
+        <f aca="false">0.06</f>
+        <v>0.06</v>
+      </c>
+      <c r="Y248" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="Z248" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AA248" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C249" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D249" s="1" t="n">
+        <f aca="false">Z248</f>
+        <v>0</v>
+      </c>
+      <c r="E249" s="1" t="n">
+        <f aca="false">AA248</f>
+        <v>0</v>
+      </c>
+      <c r="F249" s="1" t="n">
+        <f aca="false">X248</f>
+        <v>0.06</v>
+      </c>
+      <c r="G249" s="1" t="n">
+        <f aca="false">X248</f>
+        <v>0.06</v>
+      </c>
+      <c r="H249" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I249" s="1" t="n">
+        <f aca="false">U248</f>
+        <v>0.23</v>
+      </c>
+      <c r="J249" s="1" t="n">
+        <f aca="false">V248</f>
+        <v>2</v>
+      </c>
+      <c r="K249" s="1" t="n">
+        <f aca="false">S248</f>
+        <v>0.32</v>
+      </c>
+      <c r="L249" s="1" t="n">
+        <f aca="false">T248</f>
+        <v>4</v>
+      </c>
+      <c r="M249" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="N249" s="1" t="n">
+        <f aca="false">P248</f>
+        <v>0.69</v>
+      </c>
+      <c r="O249" s="1" t="n">
+        <f aca="false">Q248</f>
+        <v>6</v>
+      </c>
+      <c r="P249" s="1" t="n">
+        <f aca="false">N248</f>
+        <v>0.84</v>
+      </c>
+      <c r="Q249" s="1" t="n">
+        <f aca="false">O248</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M250" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="N250" s="1" t="n">
+        <f aca="false">P255</f>
+        <v>0.17</v>
+      </c>
+      <c r="O250" s="1" t="n">
+        <f aca="false">Q255</f>
+        <v>2</v>
+      </c>
+      <c r="P250" s="1" t="n">
+        <f aca="false">N255</f>
+        <v>0.42</v>
+      </c>
+      <c r="Q250" s="1" t="n">
+        <f aca="false">O255</f>
+        <v>2</v>
+      </c>
+      <c r="R250" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="S250" s="1" t="n">
+        <f aca="false">K255</f>
+        <v>0.31</v>
+      </c>
+      <c r="T250" s="1" t="n">
+        <f aca="false">L255</f>
+        <v>6</v>
+      </c>
+      <c r="U250" s="1" t="n">
+        <f aca="false">I255</f>
+        <v>0.13</v>
+      </c>
+      <c r="V250" s="1" t="n">
+        <f aca="false">J255</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M251" s="2" t="n">
+        <f aca="false">M261</f>
+        <v>60</v>
+      </c>
+      <c r="N251" s="1" t="n">
+        <f aca="false">P261</f>
+        <v>0.53</v>
+      </c>
+      <c r="O251" s="1" t="n">
+        <f aca="false">Q261</f>
+        <v>8</v>
+      </c>
+      <c r="P251" s="1" t="n">
+        <f aca="false">N261</f>
+        <v>0.56</v>
+      </c>
+      <c r="Q251" s="1" t="n">
+        <f aca="false">O261</f>
+        <v>7</v>
+      </c>
+      <c r="R251" s="2" t="n">
+        <f aca="false">H261</f>
+        <v>35</v>
+      </c>
+      <c r="S251" s="1" t="n">
+        <f aca="false">K261</f>
+        <v>1.19</v>
+      </c>
+      <c r="T251" s="1" t="n">
+        <f aca="false">L261</f>
+        <v>8</v>
+      </c>
+      <c r="U251" s="1" t="n">
+        <f aca="false">I261</f>
+        <v>0.1</v>
+      </c>
+      <c r="V251" s="1" t="n">
+        <f aca="false">J261</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M252" s="2" t="n">
+        <f aca="false">21+40</f>
+        <v>61</v>
+      </c>
+      <c r="N252" s="1" t="n">
+        <f aca="false">0.08+0.14</f>
+        <v>0.22</v>
+      </c>
+      <c r="O252" s="1" t="n">
+        <f aca="false">3+2</f>
+        <v>5</v>
+      </c>
+      <c r="P252" s="1" t="n">
+        <f aca="false">0.82+0.51</f>
+        <v>1.33</v>
+      </c>
+      <c r="Q252" s="1" t="n">
+        <f aca="false">9+5</f>
+        <v>14</v>
+      </c>
+      <c r="R252" s="2" t="n">
+        <f aca="false">38+8</f>
+        <v>46</v>
+      </c>
+      <c r="S252" s="1" t="n">
+        <f aca="false">1.26+0.14</f>
+        <v>1.4</v>
+      </c>
+      <c r="T252" s="1" t="n">
+        <f aca="false">6+2</f>
+        <v>8</v>
+      </c>
+      <c r="U252" s="1" t="n">
+        <f aca="false">0.64+0.26</f>
+        <v>0.9</v>
+      </c>
+      <c r="V252" s="1" t="n">
+        <f aca="false">8+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M253" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="N253" s="1" t="n">
+        <f aca="false">0.29</f>
+        <v>0.29</v>
+      </c>
+      <c r="O253" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="P253" s="1" t="n">
+        <f aca="false">0.83</f>
+        <v>0.83</v>
+      </c>
+      <c r="Q253" s="1" t="n">
+        <f aca="false">8</f>
+        <v>8</v>
+      </c>
+      <c r="R253" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="S253" s="1" t="n">
+        <f aca="false">0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="T253" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="U253" s="1" t="n">
+        <f aca="false">0.26</f>
+        <v>0.26</v>
+      </c>
+      <c r="V253" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="W253" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="X253" s="1" t="n">
+        <f aca="false">0.06</f>
+        <v>0.06</v>
+      </c>
+      <c r="Y253" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="Z253" s="1" t="n">
+        <f aca="false">0.06</f>
+        <v>0.06</v>
+      </c>
+      <c r="AA253" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H254" s="2" t="n">
+        <f aca="false">R242</f>
+        <v>4</v>
+      </c>
+      <c r="I254" s="1" t="n">
+        <f aca="false">U242</f>
+        <v>0</v>
+      </c>
+      <c r="J254" s="1" t="n">
+        <f aca="false">V242</f>
+        <v>0</v>
+      </c>
+      <c r="K254" s="1" t="n">
+        <f aca="false">S242</f>
+        <v>0.42</v>
+      </c>
+      <c r="L254" s="1" t="n">
+        <f aca="false">T242</f>
+        <v>1</v>
+      </c>
+      <c r="M254" s="2" t="n">
+        <f aca="false">M242</f>
+        <v>31</v>
+      </c>
+      <c r="N254" s="1" t="n">
+        <f aca="false">P242</f>
+        <v>0.52</v>
+      </c>
+      <c r="O254" s="1" t="n">
+        <f aca="false">Q242</f>
+        <v>8</v>
+      </c>
+      <c r="P254" s="1" t="n">
+        <f aca="false">N242</f>
+        <v>0.29</v>
+      </c>
+      <c r="Q254" s="1" t="n">
+        <f aca="false">O242</f>
+        <v>2</v>
+      </c>
+      <c r="R254" s="2" t="n">
+        <f aca="false">H242</f>
+        <v>60</v>
+      </c>
+      <c r="S254" s="1" t="n">
+        <f aca="false">K242</f>
+        <v>0.72</v>
+      </c>
+      <c r="T254" s="1" t="n">
+        <f aca="false">L242</f>
+        <v>7</v>
+      </c>
+      <c r="U254" s="1" t="n">
+        <f aca="false">I242</f>
+        <v>0.28</v>
+      </c>
+      <c r="V254" s="1" t="n">
+        <f aca="false">J242</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H255" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="I255" s="1" t="n">
+        <f aca="false">0.13</f>
+        <v>0.13</v>
+      </c>
+      <c r="J255" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="K255" s="1" t="n">
+        <f aca="false">0.31</f>
+        <v>0.31</v>
+      </c>
+      <c r="L255" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="M255" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="N255" s="1" t="n">
+        <f aca="false">0.42</f>
+        <v>0.42</v>
+      </c>
+      <c r="O255" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="P255" s="1" t="n">
+        <f aca="false">0.17</f>
+        <v>0.17</v>
+      </c>
+      <c r="Q255" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M256" s="2" t="n">
+        <f aca="false">3+26+10</f>
+        <v>39</v>
+      </c>
+      <c r="N256" s="1" t="n">
+        <f aca="false">0+0.14+0.03</f>
+        <v>0.17</v>
+      </c>
+      <c r="O256" s="1" t="n">
+        <f aca="false">0+3+2</f>
+        <v>5</v>
+      </c>
+      <c r="P256" s="1" t="n">
+        <f aca="false">0.52+0.61+0.08</f>
+        <v>1.21</v>
+      </c>
+      <c r="Q256" s="1" t="n">
+        <f aca="false">1+4+2</f>
+        <v>7</v>
+      </c>
+      <c r="R256" s="2" t="n">
+        <f aca="false">9+51</f>
+        <v>60</v>
+      </c>
+      <c r="S256" s="1" t="n">
+        <f aca="false">0.12+0.5</f>
+        <v>0.62</v>
+      </c>
+      <c r="T256" s="1" t="n">
+        <f aca="false">1+5</f>
+        <v>6</v>
+      </c>
+      <c r="U256" s="1" t="n">
+        <f aca="false">0.08</f>
+        <v>0.08</v>
+      </c>
+      <c r="V256" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C257" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="D257" s="1" t="n">
+        <f aca="false">0.09</f>
+        <v>0.09</v>
+      </c>
+      <c r="E257" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="F257" s="1" t="n">
+        <f aca="false">0.07</f>
+        <v>0.07</v>
+      </c>
+      <c r="G257" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="H257" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="I257" s="1" t="n">
+        <f aca="false">0.64</f>
+        <v>0.64</v>
+      </c>
+      <c r="J257" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="K257" s="1" t="n">
+        <f aca="false">0.59</f>
+        <v>0.59</v>
+      </c>
+      <c r="L257" s="1" t="n">
+        <f aca="false">10</f>
+        <v>10</v>
+      </c>
+      <c r="M257" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="N257" s="1" t="n">
+        <f aca="false">0.17</f>
+        <v>0.17</v>
+      </c>
+      <c r="O257" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="P257" s="1" t="n">
+        <f aca="false">0.12</f>
+        <v>0.12</v>
+      </c>
+      <c r="Q257" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H258" s="2" t="n">
+        <f aca="false">R245</f>
+        <v>32</v>
+      </c>
+      <c r="I258" s="1" t="n">
+        <f aca="false">U245</f>
+        <v>0.38</v>
+      </c>
+      <c r="J258" s="1" t="n">
+        <f aca="false">V245</f>
+        <v>4</v>
+      </c>
+      <c r="K258" s="1" t="n">
+        <f aca="false">S245</f>
+        <v>0.47</v>
+      </c>
+      <c r="L258" s="1" t="n">
+        <f aca="false">T245</f>
+        <v>6</v>
+      </c>
+      <c r="M258" s="2" t="n">
+        <f aca="false">M245</f>
+        <v>64</v>
+      </c>
+      <c r="N258" s="1" t="n">
+        <f aca="false">P245</f>
+        <v>0.84</v>
+      </c>
+      <c r="O258" s="1" t="n">
+        <f aca="false">Q245</f>
+        <v>14</v>
+      </c>
+      <c r="P258" s="1" t="n">
+        <f aca="false">N245</f>
+        <v>0.09</v>
+      </c>
+      <c r="Q258" s="1" t="n">
+        <f aca="false">O245</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H259" s="2" t="n">
+        <f aca="false">R252</f>
+        <v>46</v>
+      </c>
+      <c r="I259" s="1" t="n">
+        <f aca="false">U252</f>
+        <v>0.9</v>
+      </c>
+      <c r="J259" s="1" t="n">
+        <f aca="false">V252</f>
+        <v>9</v>
+      </c>
+      <c r="K259" s="1" t="n">
+        <f aca="false">S252</f>
+        <v>1.4</v>
+      </c>
+      <c r="L259" s="1" t="n">
+        <f aca="false">T252</f>
+        <v>8</v>
+      </c>
+      <c r="M259" s="2" t="n">
+        <f aca="false">M252</f>
+        <v>61</v>
+      </c>
+      <c r="N259" s="1" t="n">
+        <f aca="false">P252</f>
+        <v>1.33</v>
+      </c>
+      <c r="O259" s="1" t="n">
+        <f aca="false">Q252</f>
+        <v>14</v>
+      </c>
+      <c r="P259" s="1" t="n">
+        <f aca="false">N252</f>
+        <v>0.22</v>
+      </c>
+      <c r="Q259" s="1" t="n">
+        <f aca="false">O252</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H260" s="2" t="n">
+        <f aca="false">R243</f>
+        <v>25</v>
+      </c>
+      <c r="I260" s="1" t="n">
+        <f aca="false">U243</f>
+        <v>0.46</v>
+      </c>
+      <c r="J260" s="1" t="n">
+        <f aca="false">V243</f>
+        <v>1</v>
+      </c>
+      <c r="K260" s="1" t="n">
+        <f aca="false">S243</f>
+        <v>0.02</v>
+      </c>
+      <c r="L260" s="1" t="n">
+        <f aca="false">T243</f>
+        <v>1</v>
+      </c>
+      <c r="M260" s="2" t="n">
+        <f aca="false">M243</f>
+        <v>35</v>
+      </c>
+      <c r="N260" s="1" t="n">
+        <f aca="false">P243</f>
+        <v>1.06</v>
+      </c>
+      <c r="O260" s="1" t="n">
+        <f aca="false">Q243</f>
+        <v>5</v>
+      </c>
+      <c r="P260" s="1" t="n">
+        <f aca="false">N243</f>
+        <v>0</v>
+      </c>
+      <c r="Q260" s="1" t="n">
+        <f aca="false">O243</f>
+        <v>0</v>
+      </c>
+      <c r="R260" s="2" t="n">
+        <f aca="false">H243</f>
+        <v>38</v>
+      </c>
+      <c r="S260" s="1" t="n">
+        <f aca="false">K243</f>
+        <v>0.45</v>
+      </c>
+      <c r="T260" s="1" t="n">
+        <f aca="false">L243</f>
+        <v>3</v>
+      </c>
+      <c r="U260" s="1" t="n">
+        <f aca="false">I243</f>
+        <v>0.24</v>
+      </c>
+      <c r="V260" s="1" t="n">
+        <f aca="false">J243</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H261" s="2" t="n">
+        <f aca="false">35</f>
+        <v>35</v>
+      </c>
+      <c r="I261" s="1" t="n">
+        <f aca="false">0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="J261" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="K261" s="1" t="n">
+        <f aca="false">1.19</f>
+        <v>1.19</v>
+      </c>
+      <c r="L261" s="1" t="n">
+        <f aca="false">8</f>
+        <v>8</v>
+      </c>
+      <c r="M261" s="2" t="n">
+        <f aca="false">33+27</f>
+        <v>60</v>
+      </c>
+      <c r="N261" s="1" t="n">
+        <f aca="false">0.52+0.04</f>
+        <v>0.56</v>
+      </c>
+      <c r="O261" s="1" t="n">
+        <f aca="false">4+3</f>
+        <v>7</v>
+      </c>
+      <c r="P261" s="1" t="n">
+        <f aca="false">0.09+0.44</f>
+        <v>0.53</v>
+      </c>
+      <c r="Q261" s="1" t="n">
+        <f aca="false">3+5</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="10" t="n">
+        <v>14</v>
+      </c>
+      <c r="B262" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C262" s="18" t="n">
+        <f aca="false">W271</f>
+        <v>10</v>
+      </c>
+      <c r="D262" s="18" t="n">
+        <f aca="false">Z271</f>
+        <v>0</v>
+      </c>
+      <c r="E262" s="18" t="n">
+        <f aca="false">AA271</f>
+        <v>0</v>
+      </c>
+      <c r="F262" s="18" t="n">
+        <f aca="false">X271</f>
+        <v>0.43</v>
+      </c>
+      <c r="G262" s="18" t="n">
+        <f aca="false">Y271</f>
+        <v>3</v>
+      </c>
+      <c r="H262" s="11" t="n">
+        <f aca="false">R271</f>
+        <v>58</v>
+      </c>
+      <c r="I262" s="18" t="n">
+        <f aca="false">U271</f>
+        <v>0.64</v>
+      </c>
+      <c r="J262" s="18" t="n">
+        <f aca="false">V271</f>
+        <v>11</v>
+      </c>
+      <c r="K262" s="18" t="n">
+        <f aca="false">S271</f>
+        <v>0.65</v>
+      </c>
+      <c r="L262" s="18" t="n">
+        <f aca="false">T271</f>
+        <v>7</v>
+      </c>
+      <c r="M262" s="11" t="n">
+        <f aca="false">M271</f>
+        <v>28</v>
+      </c>
+      <c r="N262" s="18" t="n">
+        <f aca="false">P271</f>
+        <v>0.56</v>
+      </c>
+      <c r="O262" s="18" t="n">
+        <f aca="false">Q271</f>
+        <v>4</v>
+      </c>
+      <c r="P262" s="18" t="n">
+        <f aca="false">N271</f>
+        <v>0.39</v>
+      </c>
+      <c r="Q262" s="18" t="n">
+        <f aca="false">O271</f>
+        <v>2</v>
+      </c>
+      <c r="R262" s="11"/>
+      <c r="S262" s="18"/>
+      <c r="T262" s="18"/>
+      <c r="U262" s="18"/>
+      <c r="V262" s="18"/>
+      <c r="W262" s="11"/>
+      <c r="X262" s="18"/>
+      <c r="Y262" s="18"/>
+      <c r="Z262" s="18"/>
+      <c r="AA262" s="18"/>
+      <c r="AB262" s="12"/>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C263" s="1" t="n">
+        <f aca="false">W269</f>
+        <v>50</v>
+      </c>
+      <c r="D263" s="1" t="n">
+        <f aca="false">Z269</f>
+        <v>1.6</v>
+      </c>
+      <c r="E263" s="1" t="n">
+        <f aca="false">AA269</f>
+        <v>8</v>
+      </c>
+      <c r="F263" s="1" t="n">
+        <f aca="false">X269</f>
+        <v>0.45</v>
+      </c>
+      <c r="G263" s="1" t="n">
+        <f aca="false">Y269</f>
+        <v>6</v>
+      </c>
+      <c r="H263" s="2" t="n">
+        <f aca="false">R269</f>
+        <v>6</v>
+      </c>
+      <c r="I263" s="1" t="n">
+        <f aca="false">U269</f>
+        <v>0.04</v>
+      </c>
+      <c r="J263" s="1" t="n">
+        <f aca="false">V269</f>
+        <v>1</v>
+      </c>
+      <c r="K263" s="1" t="n">
+        <f aca="false">S269</f>
+        <v>0</v>
+      </c>
+      <c r="L263" s="1" t="n">
+        <f aca="false">T269</f>
+        <v>0</v>
+      </c>
+      <c r="M263" s="2" t="n">
+        <f aca="false">M269</f>
+        <v>32</v>
+      </c>
+      <c r="N263" s="1" t="n">
+        <f aca="false">P269</f>
+        <v>0.27</v>
+      </c>
+      <c r="O263" s="1" t="n">
+        <f aca="false">Q269</f>
+        <v>3</v>
+      </c>
+      <c r="P263" s="1" t="n">
+        <f aca="false">N269</f>
+        <v>0.18</v>
+      </c>
+      <c r="Q263" s="1" t="n">
+        <f aca="false">O269</f>
+        <v>3</v>
+      </c>
+      <c r="R263" s="2" t="n">
+        <f aca="false">H269</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M264" s="2" t="n">
+        <f aca="false">96</f>
+        <v>96</v>
+      </c>
+      <c r="N264" s="1" t="n">
+        <f aca="false">1.01</f>
+        <v>1.01</v>
+      </c>
+      <c r="O264" s="1" t="n">
+        <f aca="false">16</f>
+        <v>16</v>
+      </c>
+      <c r="P264" s="1" t="n">
+        <f aca="false">0.29</f>
+        <v>0.29</v>
+      </c>
+      <c r="Q264" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C265" s="1" t="n">
+        <f aca="false">W274</f>
+        <v>7</v>
+      </c>
+      <c r="D265" s="1" t="n">
+        <f aca="false">Z274</f>
+        <v>0.03</v>
+      </c>
+      <c r="E265" s="1" t="n">
+        <f aca="false">AA274</f>
+        <v>1</v>
+      </c>
+      <c r="F265" s="1" t="n">
+        <f aca="false">X274</f>
+        <v>0.17</v>
+      </c>
+      <c r="G265" s="1" t="n">
+        <f aca="false">Y274</f>
+        <v>3</v>
+      </c>
+      <c r="H265" s="2" t="n">
+        <f aca="false">R274</f>
+        <v>19</v>
+      </c>
+      <c r="I265" s="1" t="n">
+        <f aca="false">U274</f>
+        <v>0.63</v>
+      </c>
+      <c r="J265" s="1" t="n">
+        <f aca="false">V274</f>
+        <v>6</v>
+      </c>
+      <c r="K265" s="1" t="n">
+        <f aca="false">S274</f>
+        <v>0</v>
+      </c>
+      <c r="L265" s="1" t="n">
+        <f aca="false">T274</f>
+        <v>0</v>
+      </c>
+      <c r="M265" s="2" t="n">
+        <f aca="false">M274</f>
+        <v>69</v>
+      </c>
+      <c r="N265" s="1" t="n">
+        <f aca="false">P274</f>
+        <v>0.54</v>
+      </c>
+      <c r="O265" s="1" t="n">
+        <f aca="false">Q274</f>
+        <v>10</v>
+      </c>
+      <c r="P265" s="1" t="n">
+        <f aca="false">N274</f>
+        <v>0.09</v>
+      </c>
+      <c r="Q265" s="1" t="n">
+        <f aca="false">O274</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M266" s="2" t="n">
+        <f aca="false">15+26</f>
+        <v>41</v>
+      </c>
+      <c r="N266" s="1" t="n">
+        <f aca="false">0.03+0</f>
+        <v>0.03</v>
+      </c>
+      <c r="O266" s="1" t="n">
+        <f aca="false">1+0</f>
+        <v>1</v>
+      </c>
+      <c r="P266" s="1" t="n">
+        <f aca="false">0.7+1.02</f>
+        <v>1.72</v>
+      </c>
+      <c r="Q266" s="1" t="n">
+        <f aca="false">3+6</f>
+        <v>9</v>
+      </c>
+      <c r="R266" s="2" t="n">
+        <f aca="false">40+15</f>
+        <v>55</v>
+      </c>
+      <c r="S266" s="1" t="n">
+        <f aca="false">0.43+0</f>
+        <v>0.43</v>
+      </c>
+      <c r="T266" s="1" t="n">
+        <f aca="false">3+0</f>
+        <v>3</v>
+      </c>
+      <c r="U266" s="1" t="n">
+        <f aca="false">1.03+0.07</f>
+        <v>1.1</v>
+      </c>
+      <c r="V266" s="1" t="n">
+        <f aca="false">7+2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H267" s="2" t="n">
+        <f aca="false">36</f>
+        <v>36</v>
+      </c>
+      <c r="I267" s="1" t="n">
+        <f aca="false">0.29</f>
+        <v>0.29</v>
+      </c>
+      <c r="J267" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="K267" s="1" t="n">
+        <f aca="false">0.47</f>
+        <v>0.47</v>
+      </c>
+      <c r="L267" s="1" t="n">
+        <f aca="false">8</f>
+        <v>8</v>
+      </c>
+      <c r="M267" s="2" t="n">
+        <f aca="false">60</f>
+        <v>60</v>
+      </c>
+      <c r="N267" s="1" t="n">
+        <f aca="false">0.83</f>
+        <v>0.83</v>
+      </c>
+      <c r="O267" s="1" t="n">
+        <f aca="false">7</f>
+        <v>7</v>
+      </c>
+      <c r="P267" s="1" t="n">
+        <f aca="false">0.73</f>
+        <v>0.73</v>
+      </c>
+      <c r="Q267" s="1" t="n">
+        <f aca="false">7</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M268" s="2" t="n">
+        <f aca="false">M267</f>
+        <v>60</v>
+      </c>
+      <c r="N268" s="1" t="n">
+        <f aca="false">P267</f>
+        <v>0.73</v>
+      </c>
+      <c r="O268" s="1" t="n">
+        <f aca="false">Q267</f>
+        <v>7</v>
+      </c>
+      <c r="P268" s="1" t="n">
+        <f aca="false">N267</f>
+        <v>0.83</v>
+      </c>
+      <c r="Q268" s="1" t="n">
+        <f aca="false">O267</f>
+        <v>7</v>
+      </c>
+      <c r="R268" s="2" t="n">
+        <f aca="false">H267</f>
+        <v>36</v>
+      </c>
+      <c r="S268" s="1" t="n">
+        <f aca="false">K267</f>
+        <v>0.47</v>
+      </c>
+      <c r="T268" s="1" t="n">
+        <f aca="false">L267</f>
+        <v>8</v>
+      </c>
+      <c r="U268" s="1" t="n">
+        <f aca="false">I267</f>
+        <v>0.29</v>
+      </c>
+      <c r="V268" s="1" t="n">
+        <f aca="false">J267</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H269" s="2" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="I269" s="1" t="n">
+        <f aca="false">0.02</f>
+        <v>0.02</v>
+      </c>
+      <c r="J269" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K269" s="1" t="n">
+        <f aca="false">0.08</f>
+        <v>0.08</v>
+      </c>
+      <c r="L269" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="M269" s="2" t="n">
+        <f aca="false">22+10</f>
+        <v>32</v>
+      </c>
+      <c r="N269" s="1" t="n">
+        <f aca="false">0.18+0</f>
+        <v>0.18</v>
+      </c>
+      <c r="O269" s="1" t="n">
+        <f aca="false">3+0</f>
+        <v>3</v>
+      </c>
+      <c r="P269" s="1" t="n">
+        <f aca="false">0.15+0.12</f>
+        <v>0.27</v>
+      </c>
+      <c r="Q269" s="1" t="n">
+        <f aca="false">2+1</f>
+        <v>3</v>
+      </c>
+      <c r="R269" s="2" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="S269" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="T269" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="U269" s="1" t="n">
+        <f aca="false">0.04</f>
+        <v>0.04</v>
+      </c>
+      <c r="V269" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="W269" s="2" t="n">
+        <f aca="false">50</f>
+        <v>50</v>
+      </c>
+      <c r="X269" s="1" t="n">
+        <f aca="false">0.45</f>
+        <v>0.45</v>
+      </c>
+      <c r="Y269" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="Z269" s="1" t="n">
+        <f aca="false">1.6</f>
+        <v>1.6</v>
+      </c>
+      <c r="AA269" s="1" t="n">
+        <f aca="false">8</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M270" s="2" t="n">
+        <f aca="false">69</f>
+        <v>69</v>
+      </c>
+      <c r="N270" s="1" t="n">
+        <f aca="false">0.33</f>
+        <v>0.33</v>
+      </c>
+      <c r="O270" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="P270" s="1" t="n">
+        <f aca="false">1.31</f>
+        <v>1.31</v>
+      </c>
+      <c r="Q270" s="1" t="n">
+        <f aca="false">10</f>
+        <v>10</v>
+      </c>
+      <c r="R270" s="2" t="n">
+        <f aca="false">26</f>
+        <v>26</v>
+      </c>
+      <c r="S270" s="1" t="n">
+        <f aca="false">0.16</f>
+        <v>0.16</v>
+      </c>
+      <c r="T270" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="U270" s="1" t="n">
+        <f aca="false">0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="V270" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M271" s="2" t="n">
+        <f aca="false">28</f>
+        <v>28</v>
+      </c>
+      <c r="N271" s="1" t="n">
+        <f aca="false">0.39</f>
+        <v>0.39</v>
+      </c>
+      <c r="O271" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="P271" s="1" t="n">
+        <f aca="false">0.56</f>
+        <v>0.56</v>
+      </c>
+      <c r="Q271" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="R271" s="2" t="n">
+        <f aca="false">2+56</f>
+        <v>58</v>
+      </c>
+      <c r="S271" s="1" t="n">
+        <f aca="false">0+0.65</f>
+        <v>0.65</v>
+      </c>
+      <c r="T271" s="1" t="n">
+        <f aca="false">0+7</f>
+        <v>7</v>
+      </c>
+      <c r="U271" s="1" t="n">
+        <f aca="false">0.24+0.4</f>
+        <v>0.64</v>
+      </c>
+      <c r="V271" s="1" t="n">
+        <f aca="false">1+10</f>
+        <v>11</v>
+      </c>
+      <c r="W271" s="2" t="n">
+        <f aca="false">10</f>
+        <v>10</v>
+      </c>
+      <c r="X271" s="1" t="n">
+        <f aca="false">0.43</f>
+        <v>0.43</v>
+      </c>
+      <c r="Y271" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="Z271" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AA271" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M272" s="2" t="n">
+        <f aca="false">M264</f>
+        <v>96</v>
+      </c>
+      <c r="N272" s="1" t="n">
+        <f aca="false">P264</f>
+        <v>0.29</v>
+      </c>
+      <c r="O272" s="1" t="n">
+        <f aca="false">Q264</f>
+        <v>6</v>
+      </c>
+      <c r="P272" s="1" t="n">
+        <f aca="false">N264</f>
+        <v>1.01</v>
+      </c>
+      <c r="Q272" s="1" t="n">
+        <f aca="false">O264</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H273" s="2" t="n">
+        <f aca="false">R270</f>
+        <v>26</v>
+      </c>
+      <c r="I273" s="1" t="n">
+        <f aca="false">U270</f>
+        <v>0.2</v>
+      </c>
+      <c r="J273" s="1" t="n">
+        <f aca="false">V270</f>
+        <v>2</v>
+      </c>
+      <c r="K273" s="1" t="n">
+        <f aca="false">S270</f>
+        <v>0.16</v>
+      </c>
+      <c r="L273" s="1" t="n">
+        <f aca="false">T270</f>
+        <v>2</v>
+      </c>
+      <c r="M273" s="2" t="n">
+        <f aca="false">M270</f>
+        <v>69</v>
+      </c>
+      <c r="N273" s="1" t="n">
+        <f aca="false">P270</f>
+        <v>1.31</v>
+      </c>
+      <c r="O273" s="1" t="n">
+        <f aca="false">Q270</f>
+        <v>10</v>
+      </c>
+      <c r="P273" s="1" t="n">
+        <f aca="false">N270</f>
+        <v>0.33</v>
+      </c>
+      <c r="Q273" s="1" t="n">
+        <f aca="false">O270</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M274" s="2" t="n">
+        <f aca="false">69</f>
+        <v>69</v>
+      </c>
+      <c r="N274" s="1" t="n">
+        <f aca="false">0.09</f>
+        <v>0.09</v>
+      </c>
+      <c r="O274" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="P274" s="1" t="n">
+        <f aca="false">0.54</f>
+        <v>0.54</v>
+      </c>
+      <c r="Q274" s="1" t="n">
+        <f aca="false">10</f>
+        <v>10</v>
+      </c>
+      <c r="R274" s="2" t="n">
+        <f aca="false">19</f>
+        <v>19</v>
+      </c>
+      <c r="S274" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="T274" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="U274" s="1" t="n">
+        <f aca="false">0.63</f>
+        <v>0.63</v>
+      </c>
+      <c r="V274" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="W274" s="2" t="n">
+        <f aca="false">7</f>
+        <v>7</v>
+      </c>
+      <c r="X274" s="1" t="n">
+        <f aca="false">0.17</f>
+        <v>0.17</v>
+      </c>
+      <c r="Y274" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="Z274" s="1" t="n">
+        <f aca="false">0.03</f>
+        <v>0.03</v>
+      </c>
+      <c r="AA274" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M275" s="2" t="n">
+        <f aca="false">M278</f>
+        <v>92</v>
+      </c>
+      <c r="N275" s="1" t="n">
+        <f aca="false">P278</f>
+        <v>1.03</v>
+      </c>
+      <c r="O275" s="1" t="n">
+        <f aca="false">Q278</f>
+        <v>14</v>
+      </c>
+      <c r="P275" s="1" t="n">
+        <f aca="false">N278</f>
+        <v>0.72</v>
+      </c>
+      <c r="Q275" s="1" t="n">
+        <f aca="false">O278</f>
+        <v>11</v>
+      </c>
+      <c r="R275" s="2" t="n">
+        <f aca="false">H278</f>
+        <v>5</v>
+      </c>
+      <c r="S275" s="1" t="n">
+        <f aca="false">K278</f>
+        <v>0.19</v>
+      </c>
+      <c r="T275" s="1" t="n">
+        <f aca="false">L278</f>
+        <v>1</v>
+      </c>
+      <c r="U275" s="1" t="n">
+        <f aca="false">I278</f>
+        <v>0</v>
+      </c>
+      <c r="V275" s="1" t="n">
+        <f aca="false">J278</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H276" s="2" t="n">
+        <f aca="false">R266</f>
+        <v>55</v>
+      </c>
+      <c r="I276" s="1" t="n">
+        <f aca="false">U266</f>
+        <v>1.1</v>
+      </c>
+      <c r="J276" s="1" t="n">
+        <f aca="false">V266</f>
+        <v>9</v>
+      </c>
+      <c r="K276" s="1" t="n">
+        <f aca="false">S266</f>
+        <v>0.43</v>
+      </c>
+      <c r="L276" s="1" t="n">
+        <f aca="false">T266</f>
+        <v>3</v>
+      </c>
+      <c r="M276" s="2" t="n">
+        <f aca="false">M266</f>
+        <v>41</v>
+      </c>
+      <c r="N276" s="1" t="n">
+        <f aca="false">P266</f>
+        <v>1.72</v>
+      </c>
+      <c r="O276" s="1" t="n">
+        <f aca="false">Q266</f>
+        <v>9</v>
+      </c>
+      <c r="P276" s="1" t="n">
+        <f aca="false">O266</f>
+        <v>1</v>
+      </c>
+      <c r="Q276" s="1" t="n">
+        <f aca="false">P266</f>
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C277" s="1" t="n">
+        <f aca="false">W280</f>
+        <v>35</v>
+      </c>
+      <c r="D277" s="1" t="n">
+        <f aca="false">Z280</f>
+        <v>0.7</v>
+      </c>
+      <c r="E277" s="1" t="n">
+        <f aca="false">AA280</f>
+        <v>2</v>
+      </c>
+      <c r="F277" s="1" t="n">
+        <f aca="false">X280</f>
+        <v>0.24</v>
+      </c>
+      <c r="G277" s="1" t="n">
+        <f aca="false">Y280</f>
+        <v>6</v>
+      </c>
+      <c r="H277" s="2" t="n">
+        <f aca="false">R280</f>
+        <v>30</v>
+      </c>
+      <c r="I277" s="1" t="n">
+        <f aca="false">U280</f>
+        <v>0.18</v>
+      </c>
+      <c r="J277" s="1" t="n">
+        <f aca="false">V280</f>
+        <v>2</v>
+      </c>
+      <c r="K277" s="1" t="n">
+        <f aca="false">S280</f>
+        <v>0.3</v>
+      </c>
+      <c r="L277" s="1" t="n">
+        <f aca="false">T280</f>
+        <v>5</v>
+      </c>
+      <c r="M277" s="2" t="n">
+        <f aca="false">M280</f>
+        <v>29</v>
+      </c>
+      <c r="N277" s="1" t="n">
+        <f aca="false">P280</f>
+        <v>0.26</v>
+      </c>
+      <c r="O277" s="1" t="n">
+        <f aca="false">Q280</f>
+        <v>4</v>
+      </c>
+      <c r="P277" s="1" t="n">
+        <f aca="false">N280</f>
+        <v>0</v>
+      </c>
+      <c r="Q277" s="1" t="n">
+        <f aca="false">O280</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H278" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I278" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="J278" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="K278" s="1" t="n">
+        <f aca="false">0.19</f>
+        <v>0.19</v>
+      </c>
+      <c r="L278" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="M278" s="2" t="n">
+        <f aca="false">80+12</f>
+        <v>92</v>
+      </c>
+      <c r="N278" s="1" t="n">
+        <f aca="false">0.7+0.02</f>
+        <v>0.72</v>
+      </c>
+      <c r="O278" s="1" t="n">
+        <f aca="false">10+1</f>
+        <v>11</v>
+      </c>
+      <c r="P278" s="1" t="n">
+        <f aca="false">1+0.03</f>
+        <v>1.03</v>
+      </c>
+      <c r="Q278" s="1" t="n">
+        <f aca="false">13+1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M279" s="2" t="n">
+        <f aca="false">33+52</f>
+        <v>85</v>
+      </c>
+      <c r="N279" s="1" t="n">
+        <f aca="false">0.13+0.25</f>
+        <v>0.38</v>
+      </c>
+      <c r="O279" s="1" t="n">
+        <f aca="false">1+7</f>
+        <v>8</v>
+      </c>
+      <c r="P279" s="1" t="n">
+        <f aca="false">0.81+0.55</f>
+        <v>1.36</v>
+      </c>
+      <c r="Q279" s="1" t="n">
+        <f aca="false">5+9</f>
+        <v>14</v>
+      </c>
+      <c r="R279" s="2" t="n">
+        <f aca="false">10</f>
+        <v>10</v>
+      </c>
+      <c r="S279" s="1" t="n">
+        <f aca="false">0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="T279" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="U279" s="1" t="n">
+        <f aca="false">0.91</f>
+        <v>0.91</v>
+      </c>
+      <c r="V279" s="1" t="n">
+        <f aca="false">7</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M280" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="N280" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="O280" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="P280" s="1" t="n">
+        <f aca="false">0.26</f>
+        <v>0.26</v>
+      </c>
+      <c r="Q280" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="R280" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="S280" s="1" t="n">
+        <f aca="false">0.3</f>
+        <v>0.3</v>
+      </c>
+      <c r="T280" s="1" t="n">
+        <f aca="false">5</f>
+        <v>5</v>
+      </c>
+      <c r="U280" s="1" t="n">
+        <f aca="false">0.18</f>
+        <v>0.18</v>
+      </c>
+      <c r="V280" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="W280" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="X280" s="1" t="n">
+        <f aca="false">0.24</f>
+        <v>0.24</v>
+      </c>
+      <c r="Y280" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="Z280" s="1" t="n">
+        <f aca="false">0.7</f>
+        <v>0.7</v>
+      </c>
+      <c r="AA280" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H281" s="2" t="n">
+        <f aca="false">R279</f>
+        <v>10</v>
+      </c>
+      <c r="I281" s="1" t="n">
+        <f aca="false">U279</f>
+        <v>0.91</v>
+      </c>
+      <c r="J281" s="1" t="n">
+        <f aca="false">V279</f>
+        <v>7</v>
+      </c>
+      <c r="K281" s="1" t="n">
+        <f aca="false">S279</f>
+        <v>0.2</v>
+      </c>
+      <c r="L281" s="1" t="n">
+        <f aca="false">T279</f>
+        <v>2</v>
+      </c>
+      <c r="M281" s="2" t="n">
+        <f aca="false">M279</f>
+        <v>85</v>
+      </c>
+      <c r="N281" s="1" t="n">
+        <f aca="false">P279</f>
+        <v>1.36</v>
+      </c>
+      <c r="O281" s="1" t="n">
+        <f aca="false">Q279</f>
+        <v>14</v>
+      </c>
+      <c r="P281" s="1" t="n">
+        <f aca="false">N279</f>
+        <v>0.38</v>
+      </c>
+      <c r="Q281" s="1" t="n">
+        <f aca="false">O279</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="B282" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C282" s="18" t="n">
+        <f aca="false">16</f>
+        <v>16</v>
+      </c>
+      <c r="D282" s="18" t="n">
+        <f aca="false">0.38</f>
+        <v>0.38</v>
+      </c>
+      <c r="E282" s="18" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="F282" s="18" t="n">
+        <f aca="false">0.12</f>
+        <v>0.12</v>
+      </c>
+      <c r="G282" s="18" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="H282" s="11" t="n">
+        <f aca="false">5+20</f>
+        <v>25</v>
+      </c>
+      <c r="I282" s="18" t="n">
+        <f aca="false">0.03+0.05</f>
+        <v>0.08</v>
+      </c>
+      <c r="J282" s="18" t="n">
+        <f aca="false">1+2</f>
+        <v>3</v>
+      </c>
+      <c r="K282" s="18" t="n">
+        <f aca="false">0.03+0.53</f>
+        <v>0.56</v>
+      </c>
+      <c r="L282" s="18" t="n">
+        <f aca="false">1+5</f>
+        <v>6</v>
+      </c>
+      <c r="M282" s="11" t="n">
+        <f aca="false">25+30</f>
+        <v>55</v>
+      </c>
+      <c r="N282" s="18" t="n">
+        <f aca="false">0.02+0.99</f>
+        <v>1.01</v>
+      </c>
+      <c r="O282" s="18" t="n">
+        <f aca="false">1+4</f>
+        <v>5</v>
+      </c>
+      <c r="P282" s="18" t="n">
+        <f aca="false">0.21+0.16</f>
+        <v>0.37</v>
+      </c>
+      <c r="Q282" s="18" t="n">
+        <f aca="false">5+2</f>
+        <v>7</v>
+      </c>
+      <c r="R282" s="11" t="n">
+        <f aca="false">11</f>
+        <v>11</v>
+      </c>
+      <c r="S282" s="18" t="n">
+        <f aca="false">0.75</f>
+        <v>0.75</v>
+      </c>
+      <c r="T282" s="18" t="n">
+        <f aca="false">5</f>
+        <v>5</v>
+      </c>
+      <c r="U282" s="18" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="V282" s="18" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="W282" s="11"/>
+      <c r="X282" s="18"/>
+      <c r="Y282" s="18"/>
+      <c r="Z282" s="18"/>
+      <c r="AA282" s="18"/>
+      <c r="AB282" s="12"/>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M283" s="2" t="n">
+        <f aca="false">30</f>
+        <v>30</v>
+      </c>
+      <c r="N283" s="1" t="n">
+        <f aca="false">0.22</f>
+        <v>0.22</v>
+      </c>
+      <c r="O283" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="P283" s="1" t="n">
+        <f aca="false">0.26</f>
+        <v>0.26</v>
+      </c>
+      <c r="Q283" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="R283" s="2" t="n">
+        <f aca="false">20</f>
+        <v>20</v>
+      </c>
+      <c r="S283" s="1" t="n">
+        <f aca="false">0.08</f>
+        <v>0.08</v>
+      </c>
+      <c r="T283" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="U283" s="1" t="n">
+        <f aca="false">0.52</f>
+        <v>0.52</v>
+      </c>
+      <c r="V283" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="W283" s="2" t="n">
+        <f aca="false">44</f>
+        <v>44</v>
+      </c>
+      <c r="X283" s="1" t="n">
+        <f aca="false">0.46</f>
+        <v>0.46</v>
+      </c>
+      <c r="Y283" s="1" t="n">
+        <f aca="false">5</f>
+        <v>5</v>
+      </c>
+      <c r="Z283" s="1" t="n">
+        <f aca="false">0.06</f>
+        <v>0.06</v>
+      </c>
+      <c r="AA283" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C284" s="1" t="n">
+        <f aca="false">W285</f>
+        <v>8</v>
+      </c>
+      <c r="D284" s="1" t="n">
+        <f aca="false">Z285</f>
+        <v>0.08</v>
+      </c>
+      <c r="E284" s="1" t="n">
+        <f aca="false">AA285</f>
+        <v>1</v>
+      </c>
+      <c r="F284" s="1" t="n">
+        <f aca="false">X285</f>
+        <v>0.2</v>
+      </c>
+      <c r="G284" s="1" t="n">
+        <f aca="false">Y285</f>
+        <v>3</v>
+      </c>
+      <c r="H284" s="2" t="n">
+        <f aca="false">R285</f>
+        <v>42</v>
+      </c>
+      <c r="I284" s="1" t="n">
+        <f aca="false">U285</f>
+        <v>1.62</v>
+      </c>
+      <c r="J284" s="1" t="n">
+        <f aca="false">V285</f>
+        <v>5</v>
+      </c>
+      <c r="K284" s="1" t="n">
+        <f aca="false">S285</f>
+        <v>0.75</v>
+      </c>
+      <c r="L284" s="1" t="n">
+        <f aca="false">T285</f>
+        <v>12</v>
+      </c>
+      <c r="M284" s="2" t="n">
+        <f aca="false">M285</f>
+        <v>46</v>
+      </c>
+      <c r="N284" s="1" t="n">
+        <f aca="false">P285</f>
+        <v>0.88</v>
+      </c>
+      <c r="O284" s="1" t="n">
+        <f aca="false">Q285</f>
+        <v>6</v>
+      </c>
+      <c r="P284" s="1" t="n">
+        <f aca="false">N285</f>
+        <v>0.4</v>
+      </c>
+      <c r="Q284" s="1" t="n">
+        <f aca="false">O285</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M285" s="2" t="n">
+        <f aca="false">46</f>
+        <v>46</v>
+      </c>
+      <c r="N285" s="1" t="n">
+        <f aca="false">0.4</f>
+        <v>0.4</v>
+      </c>
+      <c r="O285" s="1" t="n">
+        <f aca="false">5</f>
+        <v>5</v>
+      </c>
+      <c r="P285" s="1" t="n">
+        <f aca="false">0.88</f>
+        <v>0.88</v>
+      </c>
+      <c r="Q285" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="R285" s="2" t="n">
+        <f aca="false">42</f>
+        <v>42</v>
+      </c>
+      <c r="S285" s="1" t="n">
+        <f aca="false">0.75</f>
+        <v>0.75</v>
+      </c>
+      <c r="T285" s="1" t="n">
+        <f aca="false">12</f>
+        <v>12</v>
+      </c>
+      <c r="U285" s="1" t="n">
+        <f aca="false">1.62</f>
+        <v>1.62</v>
+      </c>
+      <c r="V285" s="1" t="n">
+        <f aca="false">5</f>
+        <v>5</v>
+      </c>
+      <c r="W285" s="2" t="n">
+        <f aca="false">8</f>
+        <v>8</v>
+      </c>
+      <c r="X285" s="1" t="n">
+        <f aca="false">0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="Y285" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="Z285" s="1" t="n">
+        <f aca="false">0.08</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA285" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H286" s="2" t="n">
+        <f aca="false">R292</f>
+        <v>31</v>
+      </c>
+      <c r="I286" s="1" t="n">
+        <f aca="false">U292</f>
+        <v>0.04</v>
+      </c>
+      <c r="J286" s="1" t="n">
+        <f aca="false">V292</f>
+        <v>1</v>
+      </c>
+      <c r="K286" s="1" t="n">
+        <f aca="false">S292</f>
+        <v>0.28</v>
+      </c>
+      <c r="L286" s="1" t="n">
+        <f aca="false">T292</f>
+        <v>5</v>
+      </c>
+      <c r="M286" s="2" t="n">
+        <f aca="false">M292</f>
+        <v>66</v>
+      </c>
+      <c r="N286" s="1" t="n">
+        <f aca="false">P292</f>
+        <v>1.42</v>
+      </c>
+      <c r="O286" s="1" t="n">
+        <f aca="false">Q292</f>
+        <v>11</v>
+      </c>
+      <c r="P286" s="1" t="n">
+        <f aca="false">N292</f>
+        <v>0.23</v>
+      </c>
+      <c r="Q286" s="1" t="n">
+        <f aca="false">O292</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H287" s="2" t="n">
+        <f aca="false">27</f>
+        <v>27</v>
+      </c>
+      <c r="I287" s="1" t="n">
+        <f aca="false">0.02</f>
+        <v>0.02</v>
+      </c>
+      <c r="J287" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K287" s="1" t="n">
+        <f aca="false">0.67</f>
+        <v>0.67</v>
+      </c>
+      <c r="L287" s="1" t="n">
+        <f aca="false">7</f>
+        <v>7</v>
+      </c>
+      <c r="M287" s="2" t="n">
+        <f aca="false">30+16</f>
+        <v>46</v>
+      </c>
+      <c r="N287" s="1" t="n">
+        <f aca="false">0.03+0.44</f>
+        <v>0.47</v>
+      </c>
+      <c r="O287" s="1" t="n">
+        <f aca="false">1+7</f>
+        <v>8</v>
+      </c>
+      <c r="P287" s="1" t="n">
+        <f aca="false">0.72+0.51</f>
+        <v>1.23</v>
+      </c>
+      <c r="Q287" s="1" t="n">
+        <f aca="false">4+4</f>
+        <v>8</v>
+      </c>
+      <c r="R287" s="2" t="n">
+        <f aca="false">23</f>
+        <v>23</v>
+      </c>
+      <c r="S287" s="1" t="n">
+        <f aca="false">0.27</f>
+        <v>0.27</v>
+      </c>
+      <c r="T287" s="1" t="n">
+        <f aca="false">6</f>
+        <v>6</v>
+      </c>
+      <c r="U287" s="1" t="n">
+        <f aca="false">0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="V287" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M288" s="2" t="n">
+        <f aca="false">43</f>
+        <v>43</v>
+      </c>
+      <c r="N288" s="1" t="n">
+        <f aca="false">0.14</f>
+        <v>0.14</v>
+      </c>
+      <c r="O288" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="P288" s="1" t="n">
+        <f aca="false">0.21</f>
+        <v>0.21</v>
+      </c>
+      <c r="Q288" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="R288" s="2" t="n">
+        <f aca="false">11</f>
+        <v>11</v>
+      </c>
+      <c r="S288" s="1" t="n">
+        <f aca="false">0.05</f>
+        <v>0.05</v>
+      </c>
+      <c r="T288" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="U288" s="1" t="n">
+        <f aca="false">0.82</f>
+        <v>0.82</v>
+      </c>
+      <c r="V288" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="W288" s="2" t="n">
+        <f aca="false">41</f>
+        <v>41</v>
+      </c>
+      <c r="X288" s="1" t="n">
+        <f aca="false">0.26</f>
+        <v>0.26</v>
+      </c>
+      <c r="Y288" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="Z288" s="1" t="n">
+        <f aca="false">0.6</f>
+        <v>0.6</v>
+      </c>
+      <c r="AA288" s="1" t="n">
+        <f aca="false">5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H289" s="2" t="n">
+        <f aca="false">R282</f>
+        <v>11</v>
+      </c>
+      <c r="I289" s="1" t="n">
+        <f aca="false">U282</f>
+        <v>0</v>
+      </c>
+      <c r="J289" s="1" t="n">
+        <f aca="false">V282</f>
+        <v>0</v>
+      </c>
+      <c r="K289" s="1" t="n">
+        <f aca="false">S282</f>
+        <v>0.75</v>
+      </c>
+      <c r="L289" s="1" t="n">
+        <f aca="false">T282</f>
+        <v>5</v>
+      </c>
+      <c r="M289" s="2" t="n">
+        <f aca="false">M282</f>
+        <v>55</v>
+      </c>
+      <c r="N289" s="1" t="n">
+        <f aca="false">P282</f>
+        <v>0.37</v>
+      </c>
+      <c r="O289" s="1" t="n">
+        <f aca="false">Q282</f>
+        <v>7</v>
+      </c>
+      <c r="P289" s="1" t="n">
+        <f aca="false">N282</f>
+        <v>1.01</v>
+      </c>
+      <c r="Q289" s="1" t="n">
+        <f aca="false">O282</f>
+        <v>5</v>
+      </c>
+      <c r="R289" s="2" t="n">
+        <f aca="false">H282</f>
+        <v>25</v>
+      </c>
+      <c r="S289" s="1" t="n">
+        <f aca="false">K282</f>
+        <v>0.56</v>
+      </c>
+      <c r="T289" s="1" t="n">
+        <f aca="false">L282</f>
+        <v>6</v>
+      </c>
+      <c r="U289" s="1" t="n">
+        <f aca="false">I282</f>
+        <v>0.08</v>
+      </c>
+      <c r="V289" s="1" t="n">
+        <f aca="false">J282</f>
+        <v>3</v>
+      </c>
+      <c r="W289" s="2" t="n">
+        <f aca="false">C282</f>
+        <v>16</v>
+      </c>
+      <c r="X289" s="1" t="n">
+        <f aca="false">F282</f>
+        <v>0.12</v>
+      </c>
+      <c r="Y289" s="1" t="n">
+        <f aca="false">G282</f>
+        <v>4</v>
+      </c>
+      <c r="Z289" s="1" t="n">
+        <f aca="false">D282</f>
+        <v>0.38</v>
+      </c>
+      <c r="AA289" s="1" t="n">
+        <f aca="false">E282</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C290" s="1" t="n">
+        <f aca="false">W288</f>
+        <v>41</v>
+      </c>
+      <c r="D290" s="1" t="n">
+        <f aca="false">Z288</f>
+        <v>0.6</v>
+      </c>
+      <c r="E290" s="1" t="n">
+        <f aca="false">AA288</f>
+        <v>5</v>
+      </c>
+      <c r="F290" s="1" t="n">
+        <f aca="false">X288</f>
+        <v>0.26</v>
+      </c>
+      <c r="G290" s="1" t="n">
+        <f aca="false">Y288</f>
+        <v>4</v>
+      </c>
+      <c r="H290" s="2" t="n">
+        <f aca="false">R288</f>
+        <v>11</v>
+      </c>
+      <c r="I290" s="1" t="n">
+        <f aca="false">U288</f>
+        <v>0.82</v>
+      </c>
+      <c r="J290" s="1" t="n">
+        <f aca="false">V288</f>
+        <v>4</v>
+      </c>
+      <c r="K290" s="1" t="n">
+        <f aca="false">S288</f>
+        <v>0.05</v>
+      </c>
+      <c r="L290" s="1" t="n">
+        <f aca="false">T288</f>
+        <v>2</v>
+      </c>
+      <c r="M290" s="2" t="n">
+        <f aca="false">M288</f>
+        <v>43</v>
+      </c>
+      <c r="N290" s="1" t="n">
+        <f aca="false">P288</f>
+        <v>0.21</v>
+      </c>
+      <c r="O290" s="1" t="n">
+        <f aca="false">Q288</f>
+        <v>4</v>
+      </c>
+      <c r="P290" s="1" t="n">
+        <f aca="false">N288</f>
+        <v>0.14</v>
+      </c>
+      <c r="Q290" s="1" t="n">
+        <f aca="false">O288</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M291" s="2" t="n">
+        <f aca="false">M297</f>
+        <v>46</v>
+      </c>
+      <c r="N291" s="1" t="n">
+        <f aca="false">P297</f>
+        <v>0.17</v>
+      </c>
+      <c r="O291" s="1" t="n">
+        <f aca="false">Q297</f>
+        <v>4</v>
+      </c>
+      <c r="P291" s="1" t="n">
+        <f aca="false">N297</f>
+        <v>0.45</v>
+      </c>
+      <c r="Q291" s="1" t="n">
+        <f aca="false">O297</f>
+        <v>7</v>
+      </c>
+      <c r="R291" s="2" t="n">
+        <f aca="false">H297</f>
+        <v>37</v>
+      </c>
+      <c r="S291" s="1" t="n">
+        <f aca="false">K297</f>
+        <v>0.14</v>
+      </c>
+      <c r="T291" s="1" t="n">
+        <f aca="false">L297</f>
+        <v>2</v>
+      </c>
+      <c r="U291" s="1" t="n">
+        <f aca="false">I297</f>
+        <v>0.12</v>
+      </c>
+      <c r="V291" s="1" t="n">
+        <f aca="false">J297</f>
+        <v>4</v>
+      </c>
+      <c r="W291" s="2" t="n">
+        <f aca="false">C297</f>
+        <v>12</v>
+      </c>
+      <c r="X291" s="1" t="n">
+        <f aca="false">F297</f>
+        <v>0.38</v>
+      </c>
+      <c r="Y291" s="1" t="n">
+        <f aca="false">G297</f>
+        <v>5</v>
+      </c>
+      <c r="Z291" s="1" t="n">
+        <f aca="false">D297</f>
+        <v>0</v>
+      </c>
+      <c r="AA291" s="1" t="n">
+        <f aca="false">E297</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M292" s="2" t="n">
+        <f aca="false">2+64</f>
+        <v>66</v>
+      </c>
+      <c r="N292" s="1" t="n">
+        <f aca="false">0+0.23</f>
+        <v>0.23</v>
+      </c>
+      <c r="O292" s="1" t="n">
+        <f aca="false">0+6</f>
+        <v>6</v>
+      </c>
+      <c r="P292" s="1" t="n">
+        <f aca="false">0.3+1.12</f>
+        <v>1.42</v>
+      </c>
+      <c r="Q292" s="1" t="n">
+        <f aca="false">1+10</f>
+        <v>11</v>
+      </c>
+      <c r="R292" s="2" t="n">
+        <f aca="false">26+5</f>
+        <v>31</v>
+      </c>
+      <c r="S292" s="1" t="n">
+        <f aca="false">0.28</f>
+        <v>0.28</v>
+      </c>
+      <c r="T292" s="1" t="n">
+        <f aca="false">5</f>
+        <v>5</v>
+      </c>
+      <c r="U292" s="1" t="n">
+        <f aca="false">0.04</f>
+        <v>0.04</v>
+      </c>
+      <c r="V292" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M293" s="2" t="n">
+        <f aca="false">24</f>
+        <v>24</v>
+      </c>
+      <c r="N293" s="1" t="n">
+        <f aca="false">0.06</f>
+        <v>0.06</v>
+      </c>
+      <c r="O293" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="P293" s="1" t="n">
+        <f aca="false">0.4</f>
+        <v>0.4</v>
+      </c>
+      <c r="Q293" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="R293" s="2" t="n">
+        <f aca="false">11</f>
+        <v>11</v>
+      </c>
+      <c r="S293" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="T293" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="U293" s="1" t="n">
+        <f aca="false">0.21</f>
+        <v>0.21</v>
+      </c>
+      <c r="V293" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="W293" s="2" t="n">
+        <f aca="false">59</f>
+        <v>59</v>
+      </c>
+      <c r="X293" s="1" t="n">
+        <f aca="false">0.16</f>
+        <v>0.16</v>
+      </c>
+      <c r="Y293" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="Z293" s="1" t="n">
+        <f aca="false">1.26</f>
+        <v>1.26</v>
+      </c>
+      <c r="AA293" s="1" t="n">
+        <f aca="false">12</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M294" s="2" t="n">
+        <f aca="false">15</f>
+        <v>15</v>
+      </c>
+      <c r="N294" s="1" t="n">
+        <f aca="false">0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="O294" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="P294" s="1" t="n">
+        <f aca="false">0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="Q294" s="1" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+      <c r="R294" s="2" t="n">
+        <f aca="false">16+14</f>
+        <v>30</v>
+      </c>
+      <c r="S294" s="1" t="n">
+        <f aca="false">0+0.03</f>
+        <v>0.03</v>
+      </c>
+      <c r="T294" s="1" t="n">
+        <f aca="false">0+1</f>
+        <v>1</v>
+      </c>
+      <c r="U294" s="1" t="n">
+        <f aca="false">0.15+0</f>
+        <v>0.15</v>
+      </c>
+      <c r="V294" s="1" t="n">
+        <f aca="false">2+0</f>
+        <v>2</v>
+      </c>
+      <c r="W294" s="2" t="n">
+        <f aca="false">27+21+3</f>
+        <v>51</v>
+      </c>
+      <c r="X294" s="1" t="n">
+        <f aca="false">0.47</f>
+        <v>0.47</v>
+      </c>
+      <c r="Y294" s="1" t="n">
+        <f aca="false">7</f>
+        <v>7</v>
+      </c>
+      <c r="Z294" s="1" t="n">
+        <f aca="false">1.12</f>
+        <v>1.12</v>
+      </c>
+      <c r="AA294" s="1" t="n">
+        <f aca="false">10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H295" s="2" t="n">
+        <f aca="false">39</f>
+        <v>39</v>
+      </c>
+      <c r="I295" s="1" t="n">
+        <f aca="false">0.23</f>
+        <v>0.23</v>
+      </c>
+      <c r="J295" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="K295" s="1" t="n">
+        <f aca="false">0.47</f>
+        <v>0.47</v>
+      </c>
+      <c r="L295" s="1" t="n">
+        <f aca="false">8</f>
+        <v>8</v>
+      </c>
+      <c r="M295" s="2" t="n">
+        <f aca="false">55+2</f>
+        <v>57</v>
+      </c>
+      <c r="N295" s="1" t="n">
+        <f aca="false">0.65</f>
+        <v>0.65</v>
+      </c>
+      <c r="O295" s="1" t="n">
+        <f aca="false">8</f>
+        <v>8</v>
+      </c>
+      <c r="P295" s="1" t="n">
+        <f aca="false">0.46</f>
+        <v>0.46</v>
+      </c>
+      <c r="Q295" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C296" s="1" t="n">
+        <f aca="false">W293</f>
+        <v>59</v>
+      </c>
+      <c r="D296" s="1" t="n">
+        <f aca="false">Z293</f>
+        <v>1.26</v>
+      </c>
+      <c r="E296" s="1" t="n">
+        <f aca="false">AA293</f>
+        <v>12</v>
+      </c>
+      <c r="F296" s="1" t="n">
+        <f aca="false">X293</f>
+        <v>0.16</v>
+      </c>
+      <c r="G296" s="1" t="n">
+        <f aca="false">Y293</f>
+        <v>3</v>
+      </c>
+      <c r="H296" s="2" t="n">
+        <f aca="false">R293</f>
+        <v>11</v>
+      </c>
+      <c r="I296" s="1" t="n">
+        <f aca="false">U293</f>
+        <v>0.21</v>
+      </c>
+      <c r="J296" s="1" t="n">
+        <f aca="false">V293</f>
+        <v>3</v>
+      </c>
+      <c r="K296" s="1" t="n">
+        <f aca="false">S293</f>
+        <v>0</v>
+      </c>
+      <c r="L296" s="1" t="n">
+        <f aca="false">T293</f>
+        <v>0</v>
+      </c>
+      <c r="M296" s="2" t="n">
+        <f aca="false">M293</f>
+        <v>24</v>
+      </c>
+      <c r="N296" s="1" t="n">
+        <f aca="false">P293</f>
+        <v>0.4</v>
+      </c>
+      <c r="O296" s="1" t="n">
+        <f aca="false">Q293</f>
+        <v>3</v>
+      </c>
+      <c r="P296" s="1" t="n">
+        <f aca="false">N293</f>
+        <v>0.06</v>
+      </c>
+      <c r="Q296" s="1" t="n">
+        <f aca="false">O293</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C297" s="1" t="n">
+        <f aca="false">12</f>
+        <v>12</v>
+      </c>
+      <c r="D297" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E297" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="F297" s="1" t="n">
+        <f aca="false">0.38</f>
+        <v>0.38</v>
+      </c>
+      <c r="G297" s="1" t="n">
+        <f aca="false">5</f>
+        <v>5</v>
+      </c>
+      <c r="H297" s="2" t="n">
+        <f aca="false">37</f>
+        <v>37</v>
+      </c>
+      <c r="I297" s="1" t="n">
+        <f aca="false">0.12</f>
+        <v>0.12</v>
+      </c>
+      <c r="J297" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+      <c r="K297" s="1" t="n">
+        <f aca="false">0.14</f>
+        <v>0.14</v>
+      </c>
+      <c r="L297" s="1" t="n">
+        <f aca="false">2</f>
+        <v>2</v>
+      </c>
+      <c r="M297" s="2" t="n">
+        <f aca="false">46</f>
+        <v>46</v>
+      </c>
+      <c r="N297" s="1" t="n">
+        <f aca="false">0.45</f>
+        <v>0.45</v>
+      </c>
+      <c r="O297" s="1" t="n">
+        <f aca="false">7</f>
+        <v>7</v>
+      </c>
+      <c r="P297" s="1" t="n">
+        <f aca="false">0.17</f>
+        <v>0.17</v>
+      </c>
+      <c r="Q297" s="1" t="n">
+        <f aca="false">4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C298" s="1" t="n">
+        <f aca="false">W283</f>
+        <v>44</v>
+      </c>
+      <c r="D298" s="1" t="n">
+        <f aca="false">Z283</f>
+        <v>0.06</v>
+      </c>
+      <c r="E298" s="1" t="n">
+        <f aca="false">AA283</f>
+        <v>1</v>
+      </c>
+      <c r="F298" s="1" t="n">
+        <f aca="false">X283</f>
+        <v>0.46</v>
+      </c>
+      <c r="G298" s="1" t="n">
+        <f aca="false">Y283</f>
+        <v>5</v>
+      </c>
+      <c r="H298" s="2" t="n">
+        <f aca="false">R283</f>
+        <v>20</v>
+      </c>
+      <c r="I298" s="1" t="n">
+        <f aca="false">U283</f>
+        <v>0.52</v>
+      </c>
+      <c r="J298" s="1" t="n">
+        <f aca="false">V283</f>
+        <v>4</v>
+      </c>
+      <c r="K298" s="1" t="n">
+        <f aca="false">S283</f>
+        <v>0.08</v>
+      </c>
+      <c r="L298" s="1" t="n">
+        <f aca="false">T283</f>
+        <v>2</v>
+      </c>
+      <c r="M298" s="2" t="n">
+        <f aca="false">M283</f>
+        <v>30</v>
+      </c>
+      <c r="N298" s="1" t="n">
+        <f aca="false">P283</f>
+        <v>0.26</v>
+      </c>
+      <c r="O298" s="1" t="n">
+        <f aca="false">Q283</f>
+        <v>3</v>
+      </c>
+      <c r="P298" s="1" t="n">
+        <f aca="false">N283</f>
+        <v>0.22</v>
+      </c>
+      <c r="Q298" s="1" t="n">
+        <f aca="false">O283</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H299" s="2" t="n">
+        <f aca="false">R287</f>
+        <v>23</v>
+      </c>
+      <c r="I299" s="1" t="n">
+        <f aca="false">U287</f>
+        <v>0.25</v>
+      </c>
+      <c r="J299" s="1" t="n">
+        <f aca="false">V287</f>
+        <v>4</v>
+      </c>
+      <c r="K299" s="1" t="n">
+        <f aca="false">S287</f>
+        <v>0.27</v>
+      </c>
+      <c r="L299" s="1" t="n">
+        <f aca="false">T287</f>
+        <v>6</v>
+      </c>
+      <c r="M299" s="2" t="n">
+        <f aca="false">M287</f>
+        <v>46</v>
+      </c>
+      <c r="N299" s="1" t="n">
+        <f aca="false">P287</f>
+        <v>1.23</v>
+      </c>
+      <c r="O299" s="1" t="n">
+        <f aca="false">Q287</f>
+        <v>8</v>
+      </c>
+      <c r="P299" s="1" t="n">
+        <f aca="false">N287</f>
+        <v>0.47</v>
+      </c>
+      <c r="Q299" s="1" t="n">
+        <f aca="false">O287</f>
+        <v>8</v>
+      </c>
+      <c r="R299" s="2" t="n">
+        <f aca="false">H287</f>
+        <v>27</v>
+      </c>
+      <c r="S299" s="1" t="n">
+        <f aca="false">K287</f>
+        <v>0.67</v>
+      </c>
+      <c r="T299" s="1" t="n">
+        <f aca="false">L287</f>
+        <v>7</v>
+      </c>
+      <c r="U299" s="1" t="n">
+        <f aca="false">I287</f>
+        <v>0.02</v>
+      </c>
+      <c r="V299" s="1" t="n">
+        <f aca="false">J287</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M300" s="2" t="n">
+        <f aca="false">M295</f>
+        <v>57</v>
+      </c>
+      <c r="N300" s="1" t="n">
+        <f aca="false">P295</f>
+        <v>0.46</v>
+      </c>
+      <c r="O300" s="1" t="n">
+        <f aca="false">Q295</f>
+        <v>4</v>
+      </c>
+      <c r="P300" s="1" t="n">
+        <f aca="false">N295</f>
+        <v>0.65</v>
+      </c>
+      <c r="Q300" s="1" t="n">
+        <f aca="false">O295</f>
+        <v>8</v>
+      </c>
+      <c r="R300" s="2" t="n">
+        <f aca="false">H295</f>
+        <v>39</v>
+      </c>
+      <c r="S300" s="1" t="n">
+        <f aca="false">K295</f>
+        <v>0.47</v>
+      </c>
+      <c r="T300" s="1" t="n">
+        <f aca="false">L295</f>
+        <v>8</v>
+      </c>
+      <c r="U300" s="1" t="n">
+        <f aca="false">I295</f>
+        <v>0.23</v>
+      </c>
+      <c r="V300" s="1" t="n">
+        <f aca="false">J295</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C301" s="1" t="n">
+        <f aca="false">W294</f>
+        <v>51</v>
+      </c>
+      <c r="D301" s="1" t="n">
+        <f aca="false">Z294</f>
+        <v>1.12</v>
+      </c>
+      <c r="E301" s="1" t="n">
+        <f aca="false">AA294</f>
+        <v>10</v>
+      </c>
+      <c r="F301" s="1" t="n">
+        <f aca="false">X294</f>
+        <v>0.47</v>
+      </c>
+      <c r="G301" s="1" t="n">
+        <f aca="false">Y294</f>
+        <v>7</v>
+      </c>
+      <c r="H301" s="2" t="n">
+        <f aca="false">R294</f>
+        <v>30</v>
+      </c>
+      <c r="I301" s="1" t="n">
+        <f aca="false">U294</f>
+        <v>0.15</v>
+      </c>
+      <c r="J301" s="1" t="n">
+        <f aca="false">V294</f>
+        <v>2</v>
+      </c>
+      <c r="K301" s="1" t="n">
+        <f aca="false">S294</f>
+        <v>0.03</v>
+      </c>
+      <c r="L301" s="1" t="n">
+        <f aca="false">T294</f>
+        <v>1</v>
+      </c>
+      <c r="M301" s="2" t="n">
+        <f aca="false">M294</f>
+        <v>15</v>
+      </c>
+      <c r="N301" s="1" t="n">
+        <f aca="false">P294</f>
+        <v>0.2</v>
+      </c>
+      <c r="O301" s="1" t="n">
+        <f aca="false">Q294</f>
+        <v>3</v>
+      </c>
+      <c r="P301" s="1" t="n">
+        <f aca="false">N294</f>
+        <v>0.2</v>
+      </c>
+      <c r="Q301" s="1" t="n">
+        <f aca="false">O294</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="18"/>
+      <c r="B302" s="18"/>
+      <c r="C302" s="18"/>
+      <c r="D302" s="18"/>
+      <c r="E302" s="18"/>
+      <c r="F302" s="18"/>
+      <c r="G302" s="18"/>
+      <c r="H302" s="11"/>
+      <c r="I302" s="18"/>
+      <c r="J302" s="18"/>
+      <c r="K302" s="18"/>
+      <c r="L302" s="18"/>
+      <c r="M302" s="11"/>
+      <c r="N302" s="18"/>
+      <c r="O302" s="18"/>
+      <c r="P302" s="18"/>
+      <c r="Q302" s="18"/>
+      <c r="R302" s="11"/>
+      <c r="S302" s="18"/>
+      <c r="T302" s="18"/>
+      <c r="U302" s="18"/>
+      <c r="V302" s="18"/>
+      <c r="W302" s="11"/>
+      <c r="X302" s="18"/>
+      <c r="Y302" s="18"/>
+      <c r="Z302" s="18"/>
+      <c r="AA302" s="18"/>
+      <c r="AB302" s="12"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB241"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>